<commit_message>
all tests passing !!!
</commit_message>
<xml_diff>
--- a/tests/resources/test_data_query.xlsx
+++ b/tests/resources/test_data_query.xlsx
@@ -28,7 +28,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -39,6 +39,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFBF00"/>
         <bgColor rgb="00FFBF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -54,9 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -622,7 +629,7 @@
           <t>SoT</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>3067</v>
       </c>
     </row>
@@ -637,7 +644,7 @@
           <t>A11</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
         <v>89</v>
       </c>
     </row>
@@ -652,7 +659,7 @@
           <t>A13</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
         <v>89809</v>
       </c>
     </row>
@@ -667,7 +674,7 @@
           <t>F9</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2" t="n">
         <v>87879</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test refactor complete. All tests passing or ignored as necessary
</commit_message>
<xml_diff>
--- a/tests/resources/test_data_query.xlsx
+++ b/tests/resources/test_data_query.xlsx
@@ -28,18 +28,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFBF00"/>
-        <bgColor rgb="00FFBF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -60,10 +54,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -361,7 +354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,76 +382,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RPE</t>
+          <t>HSMRPG</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SoT</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>HSMRPG</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>A11</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>8900</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RPE</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>78</v>
+      <c r="C2" s="1" t="n">
+        <v>2739.7</v>
       </c>
     </row>
   </sheetData>
@@ -472,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,86 +433,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RPE</t>
+          <t>HSMRPG</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SoT</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>md</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>HSMRPG</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>A11</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>md</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>md</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RPE</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>md</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>md</t>
-        </is>
+      <c r="C2" s="1" t="n">
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,76 +484,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RPE</t>
+          <t>Rail Group</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SoT</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>3067</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>A11</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>89809</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RPE</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>87879</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4345</v>
+      <c r="C2" t="n">
+        <v>1378.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>